<commit_message>
Changed BOM to fix resistor labels
</commit_message>
<xml_diff>
--- a/bom/BPS-MinionShield BOM.xlsx
+++ b/bom/BPS-MinionShield BOM.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lakshaygupta/Documents/LHR/Battery Box Boards/BPS-MinionShieldPCB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lakshaygupta/Documents/LHR/Battery Box Boards/BPS-MinionShieldPCB/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3E7CF46-C0DB-C144-9F46-488F14F6E5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DD29B9-B1D7-1647-9F54-3239BF3F67F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="2140" windowWidth="27640" windowHeight="16280" xr2:uid="{84E0FB22-9331-CB48-B959-F897929F346D}"/>
+    <workbookView xWindow="340" yWindow="1200" windowWidth="27640" windowHeight="16280" xr2:uid="{84E0FB22-9331-CB48-B959-F897929F346D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,12 +35,141 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+  <si>
+    <t>Mftr Part Number</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Total Price</t>
+  </si>
+  <si>
+    <t>C3, C4, C5, C6, C7, C8, C9, C10, C11, C12, C13, C14, C15, C16, C17, C18</t>
+  </si>
+  <si>
+    <t>C1, C2</t>
+  </si>
+  <si>
+    <t>R2, R3, R4, R5, R10, R11, R12, R13, R18, R19, R20, R21, R26, R27, R28, R29</t>
+  </si>
+  <si>
+    <t>R6, R7, R8, R9, R14, R15, R16, R17, R22, R23, R24, R25, R30, R31, R32, R33</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>FB1, FB2, FB3, FB4, FB5, FB6, FB7, FB8, FB9, FB10, FB11, FB12, FB13, FB14, FB15, FB16, FB17, FB18</t>
+  </si>
+  <si>
+    <t>PCB Reference</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>PowerLed1</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>875-HZ0805B222R-10</t>
+  </si>
+  <si>
+    <t>710-150080VS75000</t>
+  </si>
+  <si>
+    <t>603-RT0603FRE074K7L</t>
+  </si>
+  <si>
+    <t>80-C0805C105Z4V</t>
+  </si>
+  <si>
+    <t>603-RT0603FRE0710KL</t>
+  </si>
+  <si>
+    <t>455-2146-ND</t>
+  </si>
+  <si>
+    <t>J1, J2</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>Ferrite Bead</t>
+  </si>
+  <si>
+    <t>Testpoint</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -63,13 +192,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,12 +520,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7722F65-3E41-E340-9F48-7579F066D735}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="90" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2">
+        <f t="shared" ref="G2:G11" si="0">B2*E2</f>
+        <v>1.264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="3">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.752</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="4">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4039999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A7" r:id="rId1" display="https://www.mouser.com/ProductDetail/875-HZ0805B222R-10" xr:uid="{AA3F8761-1213-AB49-AE61-6F2349E973D7}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://www.mouser.com/ProductDetail/710-150080VS75000" xr:uid="{E3CE51F6-C90C-0F49-BADF-7D9F69CD5388}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://www.mouser.com/ProductDetail/603-RT0603FRE074K7L" xr:uid="{09002B95-A781-4242-8B36-855F89E4B95B}"/>
+    <hyperlink ref="A2" r:id="rId4" display="https://www.mouser.com/ProductDetail/80-C0805C105Z4V" xr:uid="{ABE08051-1745-5245-9870-621BBACCC529}"/>
+    <hyperlink ref="A5" r:id="rId5" display="https://www.mouser.com/ProductDetail/603-RT0603FRE0710KL" xr:uid="{6C5E0E15-6BDD-C247-8D2C-DCCC9B96DC3A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>